<commit_message>
The first version of API functions are added
</commit_message>
<xml_diff>
--- a/Examples/Net3/Result/Net3-Example.xlsx
+++ b/Examples/Net3/Result/Net3-Example.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Examples/Net3/Result</t>
+          <t>C:\Users\naeim\OneDrive\Desktop\REWET\Examples\Net3\Result</t>
         </is>
       </c>
     </row>
@@ -500,7 +500,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Examples/Net3/RunFiles</t>
+          <t>C:\Users\naeim\OneDrive\Desktop\REWET\Examples\Net3\RunFiles</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Examples/Net3/net3.inp</t>
+          <t>C:\Users\naeim\OneDrive\Desktop\REWET\Examples\Net3\Net3.inp</t>
         </is>
       </c>
     </row>
@@ -628,7 +628,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Examples/Net3/list.xlsx</t>
+          <t>C:\Users\naeim\OneDrive\Desktop\REWET\test\test_data\10_day_Net3_No_restoration\test_list.xlsx</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Examples/Net3/Damages</t>
+          <t>C:\Users\naeim\OneDrive\Desktop\REWET\test\test_data\10_day_Net3_No_restoration\Damages</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="B23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -940,7 +940,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Examples/Net3/config.txt</t>
+          <t>C:\Users\naeim\OneDrive\Desktop\REWET\Examples\Net3\config.txt</t>
         </is>
       </c>
     </row>

</xml_diff>